<commit_message>
Misspelling in "access control"
</commit_message>
<xml_diff>
--- a/SQL-DBA-Custom-Roles.xlsx
+++ b/SQL-DBA-Custom-Roles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sammes_microsoft_com/Documents/GBB SHARE/customer presentation/Elevance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/kiraymon_microsoft_com/Documents/Source/GitHub/SQL-Least-Privilege-Access-Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="681" documentId="8_{39A0F22A-81F8-4386-B19D-37792C91B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41A7B53D-EFEB-4159-A973-75EFC4927703}"/>
+  <xr:revisionPtr revIDLastSave="683" documentId="8_{39A0F22A-81F8-4386-B19D-37792C91B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92EB8899-3372-4CE9-A2F8-588B65296EE0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="396" xr2:uid="{9D03CC2A-540D-47FF-8FB3-9E4348DF9561}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="30210" windowHeight="18855" tabRatio="396" xr2:uid="{9D03CC2A-540D-47FF-8FB3-9E4348DF9561}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$N$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="341">
   <si>
     <t>DROP SCHEMA</t>
   </si>
@@ -1346,9 +1345,6 @@
   </si>
   <si>
     <t>PENDING: !!! dbcc errorlog !!!</t>
-  </si>
-  <si>
-    <t>acces control</t>
   </si>
   <si>
     <t>GRANT 	VIEW ANY ERROR LOG</t>
@@ -1866,7 +1862,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57F65908-FD20-4E10-9F0E-B07DAD0D797C}" name="Table1" displayName="Table1" ref="A1:M81" totalsRowShown="0">
-  <autoFilter ref="A1:M81" xr:uid="{57F65908-FD20-4E10-9F0E-B07DAD0D797C}"/>
+  <autoFilter ref="A1:M81" xr:uid="{57F65908-FD20-4E10-9F0E-B07DAD0D797C}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="acces control"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4258994F-8041-4336-9E4E-EA2CCB2D1359}" name="Outline ID"/>
     <tableColumn id="2" xr3:uid="{EEAFABE7-59BC-45FD-9A3F-43C3A1A19A8E}" name="Category"/>
@@ -2206,32 +2208,32 @@
   <dimension ref="A1:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F72" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
+      <selection pane="bottomRight" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="53.5546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.21875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="47.21875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" style="26" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="11" max="11" width="31.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" style="15" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" customWidth="1"/>
-    <col min="16" max="16" width="34.44140625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="47.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="26" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="15" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2355,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2385,7 +2387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2415,7 +2417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2437,7 +2439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -2463,7 +2465,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -2507,7 +2509,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -2551,7 +2553,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="57.6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" ht="69" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -2565,7 +2567,7 @@
         <v>280</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>293</v>
@@ -2589,7 +2591,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -2603,7 +2605,7 @@
         <v>280</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>293</v>
@@ -2622,7 +2624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -2636,7 +2638,7 @@
         <v>280</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>293</v>
@@ -2661,7 +2663,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -2675,7 +2677,7 @@
         <v>280</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I13" t="s">
         <v>294</v>
@@ -2695,7 +2697,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -2709,7 +2711,7 @@
         <v>280</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I14" t="s">
         <v>294</v>
@@ -2727,7 +2729,7 @@
       </c>
       <c r="P14" s="16"/>
     </row>
-    <row r="15" spans="1:19" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -2741,7 +2743,7 @@
         <v>280</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I15" t="s">
         <v>294</v>
@@ -2759,7 +2761,7 @@
       </c>
       <c r="P15" s="16"/>
     </row>
-    <row r="16" spans="1:19" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -2773,7 +2775,7 @@
         <v>276</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I16" t="s">
         <v>278</v>
@@ -2796,7 +2798,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -2810,7 +2812,7 @@
         <v>276</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I17" s="29"/>
       <c r="K17" s="7"/>
@@ -2828,7 +2830,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>276</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I18" s="29"/>
       <c r="K18" s="7"/>
@@ -2860,7 +2862,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -2874,7 +2876,7 @@
         <v>276</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I19" s="29"/>
       <c r="K19" s="7"/>
@@ -2892,7 +2894,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -2906,7 +2908,7 @@
         <v>276</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I20" s="29"/>
       <c r="K20" s="7"/>
@@ -2924,7 +2926,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -2938,7 +2940,7 @@
         <v>276</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I21" s="29"/>
       <c r="K21" s="7"/>
@@ -2962,7 +2964,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -2976,7 +2978,7 @@
         <v>276</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I22" s="29"/>
       <c r="K22" s="7"/>
@@ -3000,7 +3002,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -3014,7 +3016,7 @@
         <v>276</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I23" s="29"/>
       <c r="K23" s="7"/>
@@ -3038,7 +3040,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -3052,7 +3054,7 @@
         <v>276</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I24" s="29"/>
       <c r="K24" s="7"/>
@@ -3067,7 +3069,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -3081,7 +3083,7 @@
         <v>276</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I25" s="29"/>
       <c r="K25" s="7"/>
@@ -3105,7 +3107,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -3119,7 +3121,7 @@
         <v>276</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I26" s="29"/>
       <c r="K26" s="7"/>
@@ -3137,7 +3139,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>158</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>276</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I27" s="29"/>
       <c r="K27" s="7"/>
@@ -3169,7 +3171,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>159</v>
       </c>
@@ -3183,7 +3185,7 @@
         <v>276</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I28" s="29"/>
       <c r="K28" s="7"/>
@@ -3198,7 +3200,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>160</v>
       </c>
@@ -3212,7 +3214,7 @@
         <v>276</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I29" s="29"/>
       <c r="K29" s="7"/>
@@ -3227,7 +3229,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -3241,7 +3243,7 @@
         <v>276</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I30" s="29"/>
       <c r="K30" s="7"/>
@@ -3256,7 +3258,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>276</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I31" s="29"/>
       <c r="K31" s="7"/>
@@ -3285,7 +3287,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -3299,7 +3301,7 @@
         <v>276</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I32" s="29"/>
       <c r="K32" s="7"/>
@@ -3320,7 +3322,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -3334,7 +3336,7 @@
         <v>276</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I33" s="29"/>
       <c r="K33" s="7"/>
@@ -3352,7 +3354,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>165</v>
       </c>
@@ -3366,7 +3368,7 @@
         <v>276</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I34" s="29"/>
       <c r="K34" s="7"/>
@@ -3384,7 +3386,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>166</v>
       </c>
@@ -3398,7 +3400,7 @@
         <v>276</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I35" s="29"/>
       <c r="K35" s="7"/>
@@ -3413,7 +3415,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>167</v>
       </c>
@@ -3427,7 +3429,7 @@
         <v>276</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I36" s="29"/>
       <c r="K36" s="7"/>
@@ -3445,7 +3447,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>168</v>
       </c>
@@ -3459,7 +3461,7 @@
         <v>276</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I37" t="s">
         <v>279</v>
@@ -3485,7 +3487,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -3499,7 +3501,7 @@
         <v>276</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I38" t="s">
         <v>279</v>
@@ -3525,7 +3527,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>170</v>
       </c>
@@ -3539,7 +3541,7 @@
         <v>276</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I39" t="s">
         <v>279</v>
@@ -3559,7 +3561,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -3573,7 +3575,7 @@
         <v>276</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I40" t="s">
         <v>281</v>
@@ -3593,7 +3595,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>172</v>
       </c>
@@ -3607,7 +3609,7 @@
         <v>280</v>
       </c>
       <c r="I41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K41" s="7"/>
       <c r="L41" s="4"/>
@@ -3628,7 +3630,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>173</v>
       </c>
@@ -3642,7 +3644,7 @@
         <v>280</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I42" t="s">
         <v>284</v>
@@ -3664,7 +3666,7 @@
       </c>
       <c r="R42" s="16"/>
     </row>
-    <row r="43" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -3678,7 +3680,7 @@
         <v>280</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I43" t="s">
         <v>284</v>
@@ -3700,7 +3702,7 @@
       </c>
       <c r="R43" s="16"/>
     </row>
-    <row r="44" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>175</v>
       </c>
@@ -3716,7 +3718,7 @@
       <c r="K44" s="7"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="38.4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:18" ht="34.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>225</v>
       </c>
@@ -3757,7 +3759,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>226</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>227</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>233</v>
       </c>
@@ -3855,7 +3857,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>234</v>
       </c>
@@ -3889,7 +3891,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>235</v>
       </c>
@@ -3923,7 +3925,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>239</v>
       </c>
@@ -3954,7 +3956,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>248</v>
       </c>
@@ -3985,7 +3987,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>249</v>
       </c>
@@ -4019,7 +4021,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>250</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>251</v>
       </c>
@@ -4070,7 +4072,7 @@
       </c>
       <c r="O55" s="16"/>
     </row>
-    <row r="56" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>271</v>
       </c>
@@ -4102,7 +4104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
         <v>310</v>
       </c>
@@ -4138,7 +4140,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>310</v>
       </c>
@@ -4149,10 +4151,10 @@
         <v>55</v>
       </c>
       <c r="G58" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="H58" s="36" t="s">
         <v>315</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>316</v>
       </c>
       <c r="I58" s="27"/>
       <c r="J58" t="s">
@@ -4161,7 +4163,7 @@
       <c r="L58" s="4"/>
       <c r="P58" s="21"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>312</v>
       </c>
@@ -4180,7 +4182,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -4194,12 +4196,12 @@
         <v>280</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I60" s="27"/>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>276</v>
       </c>
       <c r="H61" s="37" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I61" s="27"/>
       <c r="L61" s="4"/>
@@ -4221,7 +4223,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -4239,67 +4241,67 @@
       </c>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B63" t="s">
         <v>31</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I63" s="27"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B64" t="s">
         <v>31</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I64" s="27"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="38" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B65" t="s">
         <v>31</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G65" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="I65" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="H65" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="I65" s="27" t="s">
-        <v>332</v>
-      </c>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="38" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B66" t="s">
         <v>31</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I66" s="27"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:16" ht="72.599999999999994" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -4338,9 +4340,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -4358,7 +4360,7 @@
         <v>280</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I68" s="27"/>
       <c r="J68" t="s">
@@ -4374,9 +4376,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -4391,7 +4393,7 @@
         <v>19</v>
       </c>
       <c r="G69" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I69" s="27"/>
       <c r="J69" t="s">
@@ -4404,9 +4406,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -4424,7 +4426,7 @@
         <v>280</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I70" s="27"/>
       <c r="J70" t="s">
@@ -4443,9 +4445,9 @@
         <v>267</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
@@ -4463,7 +4465,7 @@
         <v>280</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I71" s="27"/>
       <c r="J71" t="s">
@@ -4476,9 +4478,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
@@ -4496,7 +4498,7 @@
         <v>280</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I72" s="27"/>
       <c r="J72" t="s">
@@ -4509,7 +4511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -4524,7 +4526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>212</v>
       </c>
@@ -4541,11 +4543,11 @@
         <v>280</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I74" s="30"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>217</v>
       </c>
@@ -4562,11 +4564,11 @@
         <v>280</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I75" s="30"/>
     </row>
-    <row r="76" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>218</v>
       </c>
@@ -4580,12 +4582,12 @@
         <v>214</v>
       </c>
       <c r="G76" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H76" s="23"/>
       <c r="I76" s="30"/>
     </row>
-    <row r="77" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>219</v>
       </c>
@@ -4599,12 +4601,12 @@
         <v>215</v>
       </c>
       <c r="G77" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H77" s="23"/>
       <c r="I77" s="30"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>65</v>
       </c>
@@ -4616,7 +4618,7 @@
       </c>
       <c r="I78" s="27"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>66</v>
       </c>
@@ -4628,7 +4630,7 @@
       </c>
       <c r="I79" s="27"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -4640,7 +4642,7 @@
       </c>
       <c r="I80" s="27"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Started standardizing wording in columns: G: Implementation/Example K: Role/Permissions Needed
Updated column header names on
K: Role/Permission Needed
O: Permissions Least Privileged
</commit_message>
<xml_diff>
--- a/SQL-DBA-Custom-Roles.xlsx
+++ b/SQL-DBA-Custom-Roles.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/kiraymon_microsoft_com/Documents/Source/GitHub/SQL-Least-Privilege-Access-Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="8_{39A0F22A-81F8-4386-B19D-37792C91B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92EB8899-3372-4CE9-A2F8-588B65296EE0}"/>
+  <xr:revisionPtr revIDLastSave="817" documentId="8_{39A0F22A-81F8-4386-B19D-37792C91B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{201B663B-463D-4BEE-9C92-DE4B8FBDC182}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="30210" windowHeight="18855" tabRatio="396" xr2:uid="{9D03CC2A-540D-47FF-8FB3-9E4348DF9561}"/>
+    <workbookView xWindow="18255" yWindow="3255" windowWidth="32130" windowHeight="16545" tabRatio="396" xr2:uid="{9D03CC2A-540D-47FF-8FB3-9E4348DF9561}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$N$1:$R$1</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="354">
   <si>
     <t>DROP SCHEMA</t>
   </si>
@@ -157,9 +158,6 @@
     <t>TSQL Command</t>
   </si>
   <si>
-    <t>Permission needed</t>
-  </si>
-  <si>
     <t>Link to permissions doc</t>
   </si>
   <si>
@@ -169,9 +167,6 @@
     <t>Elastic Jobs (or use pipelines)</t>
   </si>
   <si>
-    <t>User user-assigned managed identity</t>
-  </si>
-  <si>
     <t>sys.event_log</t>
   </si>
   <si>
@@ -356,9 +351,6 @@
   </si>
   <si>
     <t>dbo</t>
-  </si>
-  <si>
-    <t>PERMISSIONs</t>
   </si>
   <si>
     <t>BACKUP DATABASE , BACKUP LOG</t>
@@ -1293,9 +1285,6 @@
     <t>03G</t>
   </si>
   <si>
-    <t>BREAK GLASS</t>
-  </si>
-  <si>
     <t>demo not available</t>
   </si>
   <si>
@@ -1506,9 +1495,6 @@
     <t>200_B1_A, 200_B1_B, 200_B1_C, 200_B1_D</t>
   </si>
   <si>
-    <t>access control: extend code 200_B1_B_x03C0C_test_DBA_with_db_ddlAdmin_index_Maintenance</t>
-  </si>
-  <si>
     <t>5b1</t>
   </si>
   <si>
@@ -1528,13 +1514,91 @@
   </si>
   <si>
     <t>200_B1_A, 200_B1_B, 500_B4_A</t>
+  </si>
+  <si>
+    <t>login_internal_principal_spconfigure</t>
+  </si>
+  <si>
+    <t>user_internal_principal_spconfigure</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>role_internal_principal_spconfigure</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <r>
+      <t>ALTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> SETTINGS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+ALTER SERVER ROLE [sysadmin] ADD MEMBER [login_internal_principal_spconfigure]
+GO
+ALTER SERVER ROLE [serveradmin] ADD MEMBER [login_internal_principal_spconfigure]
+GO</t>
+    </r>
+  </si>
+  <si>
+    <t>100_B1_create_Login_User</t>
+  </si>
+  <si>
+    <t>100_B2_wrapper_create_sp_configure</t>
+  </si>
+  <si>
+    <t>SQL file</t>
+  </si>
+  <si>
+    <t>Use user-assigned managed identity</t>
+  </si>
+  <si>
+    <t>Role/Permission needed</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Permissions Least Privileged</t>
+  </si>
+  <si>
+    <t>ALTER</t>
+  </si>
+  <si>
+    <t>extend code 200_B1_B_x03C0C_test_DBA_with_db_ddlAdmin_index_Maintenance</t>
+  </si>
+  <si>
+    <t>200_B1_B_x03C0C_test_DBA_with_db_ddlAdmin_index_Maintenance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1653,6 +1717,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1687,7 +1769,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1724,9 +1806,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1752,9 +1831,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1787,6 +1863,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1862,13 +1948,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57F65908-FD20-4E10-9F0E-B07DAD0D797C}" name="Table1" displayName="Table1" ref="A1:M81" totalsRowShown="0">
-  <autoFilter ref="A1:M81" xr:uid="{57F65908-FD20-4E10-9F0E-B07DAD0D797C}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="acces control"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M81" xr:uid="{57F65908-FD20-4E10-9F0E-B07DAD0D797C}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4258994F-8041-4336-9E4E-EA2CCB2D1359}" name="Outline ID"/>
     <tableColumn id="2" xr3:uid="{EEAFABE7-59BC-45FD-9A3F-43C3A1A19A8E}" name="Category"/>
@@ -1880,7 +1960,7 @@
     <tableColumn id="13" xr3:uid="{820DAE1A-1F09-49EB-9D97-D8AC5C37D36B}" name="demo code" dataDxfId="4"/>
     <tableColumn id="11" xr3:uid="{FD77081F-51B9-436F-BB4B-26984279351A}" name="Status" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{6AA74B82-BBBC-4B26-A37A-DFD35775F7EB}" name="TSQL Command"/>
-    <tableColumn id="8" xr3:uid="{F405FBD2-4CB7-4BB0-A901-B3088B3ECB3B}" name="Permission needed" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{F405FBD2-4CB7-4BB0-A901-B3088B3ECB3B}" name="Role/Permission needed" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{91E03F60-25E8-4C7D-B7FE-57077042DBEA}" name="Link to permissions doc" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{FCE70795-ED8C-4D5F-A976-6BCCBF816EBC}" name="Column1" dataDxfId="0"/>
   </tableColumns>
@@ -2211,7 +2291,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G82" sqref="G82"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,13 +2304,15 @@
     <col min="6" max="6" width="53.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="47.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="26" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="25" customWidth="1"/>
     <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="31.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="15" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="14" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" customWidth="1"/>
-    <col min="16" max="16" width="34.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2244,54 +2326,54 @@
         <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="I1" s="26" t="s">
         <v>274</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>271</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>82</v>
+      <c r="M1" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>91</v>
+        <v>350</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -2306,22 +2388,25 @@
         <v>20</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="I2" s="26"/>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -2336,28 +2421,28 @@
         <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>299</v>
+        <v>45</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>295</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2374,20 +2459,23 @@
         <v>20</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="27"/>
+        <v>44</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I4" s="26"/>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>28</v>
+        <v>347</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2404,11 +2492,14 @@
         <v>19</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="27"/>
+        <v>44</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I5" s="26"/>
       <c r="J5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>14</v>
@@ -2417,57 +2508,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>301</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>298</v>
+        <v>47</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>294</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="31" t="s">
+        <v>297</v>
+      </c>
       <c r="L6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>298</v>
+        <v>49</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>294</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L7" s="4"/>
-      <c r="P7" s="21" t="s">
-        <v>75</v>
+      <c r="P7" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="S7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -2476,42 +2571,44 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>302</v>
+        <v>300</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>298</v>
       </c>
       <c r="J8" s="12"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="15" t="s">
+      <c r="K8" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="N8" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" s="16" t="s">
+      <c r="R8" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>83</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -2520,57 +2617,59 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>95</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="I9" s="28" t="s">
-        <v>303</v>
-      </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="69" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>98</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
@@ -2581,1164 +2680,1232 @@
       <c r="L10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="15" t="s">
-        <v>110</v>
+      <c r="M10" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="O10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>99</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="P11" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="N11" s="9" t="s">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>102</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>105</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="15" t="s">
-        <v>101</v>
+      <c r="M12" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q12" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="R12" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I13" t="s">
-        <v>294</v>
-      </c>
-      <c r="K13" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="P13" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="N13" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I14" t="s">
-        <v>294</v>
-      </c>
-      <c r="K14" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="15" t="s">
-        <v>211</v>
+      <c r="M14" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="O14" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="P14" s="16"/>
-    </row>
-    <row r="15" spans="1:19" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="P14" s="15"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I15" t="s">
-        <v>294</v>
-      </c>
-      <c r="K15" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="15" t="s">
-        <v>101</v>
+      <c r="M15" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="O15" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="P15" s="16"/>
-    </row>
-    <row r="16" spans="1:19" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="P15" s="15"/>
+    </row>
+    <row r="16" spans="1:19" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I16" t="s">
-        <v>278</v>
-      </c>
-      <c r="K16" s="7"/>
+        <v>275</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="15" t="s">
-        <v>120</v>
+      <c r="M16" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>83</v>
+        <v>131</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q16" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="S16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I17" s="29"/>
-      <c r="K17" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I17" s="27"/>
+      <c r="K17" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="15" t="s">
-        <v>121</v>
+      <c r="M17" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q17" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q17" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I18" s="29"/>
-      <c r="K18" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I18" s="27"/>
+      <c r="K18" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="15" t="s">
-        <v>122</v>
+      <c r="M18" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q18" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q18" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I19" s="29"/>
-      <c r="K19" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I19" s="27"/>
+      <c r="K19" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="15" t="s">
-        <v>123</v>
+      <c r="M19" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="P19" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q19" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I20" s="29"/>
-      <c r="K20" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I20" s="27"/>
+      <c r="K20" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="15" t="s">
-        <v>135</v>
+      <c r="M20" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q20" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I21" s="29"/>
-      <c r="K21" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I21" s="27"/>
+      <c r="K21" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="15" t="s">
-        <v>136</v>
+      <c r="M21" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q21" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R21" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I22" s="29"/>
-      <c r="K22" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I22" s="27"/>
+      <c r="K22" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="15" t="s">
-        <v>139</v>
+      <c r="M22" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q22" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I23" s="29"/>
-      <c r="K23" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I23" s="27"/>
+      <c r="K23" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="15" t="s">
-        <v>146</v>
+      <c r="M23" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q23" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="O23" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I24" s="29"/>
-      <c r="K24" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I24" s="27"/>
+      <c r="K24" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="15" t="s">
-        <v>147</v>
+      <c r="M24" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G25" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I25" s="29"/>
-      <c r="K25" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I25" s="27"/>
+      <c r="K25" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="15" t="s">
-        <v>148</v>
+      <c r="M25" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q25" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="O25" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="P25" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R25" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I26" s="29"/>
-      <c r="K26" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I26" s="27"/>
+      <c r="K26" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L26" s="4"/>
-      <c r="M26" s="15" t="s">
-        <v>149</v>
+      <c r="M26" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="N26" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q26" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>155</v>
-      </c>
-      <c r="P26" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q26" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>158</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I27" s="29"/>
-      <c r="K27" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I27" s="27"/>
+      <c r="K27" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L27" s="4"/>
-      <c r="M27" s="15" t="s">
-        <v>150</v>
+      <c r="M27" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="N27" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="O27" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="P27" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>156</v>
-      </c>
-      <c r="O27" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="P27" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>159</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I28" s="29"/>
-      <c r="K28" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I28" s="27"/>
+      <c r="K28" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L28" s="4"/>
-      <c r="M28" s="15" t="s">
-        <v>181</v>
+      <c r="M28" s="14" t="s">
+        <v>178</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="O28" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="O28" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I29" s="29"/>
-      <c r="K29" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I29" s="27"/>
+      <c r="K29" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L29" s="4"/>
-      <c r="M29" s="15" t="s">
-        <v>183</v>
+      <c r="M29" s="14" t="s">
+        <v>180</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="P29" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I30" s="29"/>
-      <c r="K30" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I30" s="27"/>
+      <c r="K30" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L30" s="4"/>
-      <c r="M30" s="15" t="s">
-        <v>185</v>
+      <c r="M30" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="O30" s="16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="O30" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I31" s="29"/>
-      <c r="K31" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I31" s="27"/>
+      <c r="K31" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L31" s="4"/>
-      <c r="M31" s="15" t="s">
-        <v>188</v>
+      <c r="M31" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="P31" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I32" s="29"/>
-      <c r="K32" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I32" s="27"/>
+      <c r="K32" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L32" s="4"/>
-      <c r="M32" s="15" t="s">
-        <v>190</v>
+      <c r="M32" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="P32" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q32" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R32" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R32" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I33" s="29"/>
-      <c r="K33" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I33" s="27"/>
+      <c r="K33" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L33" s="4"/>
-      <c r="M33" s="15" t="s">
-        <v>192</v>
+      <c r="M33" s="14" t="s">
+        <v>189</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="P33" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="P33" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I34" s="29"/>
-      <c r="K34" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I34" s="27"/>
+      <c r="K34" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L34" s="4"/>
-      <c r="M34" s="15" t="s">
-        <v>195</v>
+      <c r="M34" s="14" t="s">
+        <v>192</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="P34" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q34" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="P34" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q34" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G35" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I35" s="29"/>
-      <c r="K35" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I35" s="27"/>
+      <c r="K35" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="15" t="s">
-        <v>197</v>
+      <c r="M35" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="P35" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="P35" s="19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G36" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I36" s="29"/>
-      <c r="K36" s="7"/>
+        <v>314</v>
+      </c>
+      <c r="I36" s="27"/>
+      <c r="K36" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L36" s="4"/>
-      <c r="M36" s="15" t="s">
-        <v>200</v>
+      <c r="M36" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="P36" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q36" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="P36" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q36" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G37" t="s">
+        <v>273</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="I37" t="s">
         <v>276</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I37" t="s">
-        <v>279</v>
-      </c>
-      <c r="K37" s="7"/>
+      <c r="K37" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L37" s="4"/>
-      <c r="M37" s="15" t="s">
-        <v>202</v>
+      <c r="M37" s="14" t="s">
+        <v>199</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="O37" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="P37" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q37" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R37" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="P37" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q37" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R37" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G38" t="s">
+        <v>273</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="I38" t="s">
         <v>276</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I38" t="s">
-        <v>279</v>
-      </c>
-      <c r="K38" s="7"/>
+      <c r="K38" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L38" s="4"/>
-      <c r="M38" s="15" t="s">
-        <v>205</v>
+      <c r="M38" s="14" t="s">
+        <v>202</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="O38" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="P38" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q38" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R38" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="P38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q38" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R38" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G39" t="s">
+        <v>273</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="I39" t="s">
         <v>276</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I39" t="s">
-        <v>279</v>
-      </c>
-      <c r="K39" s="7"/>
+      <c r="K39" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L39" s="4"/>
-      <c r="M39" s="15" t="s">
-        <v>207</v>
+      <c r="M39" s="14" t="s">
+        <v>204</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="P39" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q39" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+      <c r="P39" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q39" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G40" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I40" t="s">
-        <v>281</v>
-      </c>
-      <c r="K40" s="7"/>
+        <v>278</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L40" s="4"/>
-      <c r="M40" s="15" t="s">
-        <v>209</v>
+      <c r="M40" s="14" t="s">
+        <v>206</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="P40" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q40" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+      <c r="P40" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q40" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G41" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I41" t="s">
-        <v>319</v>
-      </c>
-      <c r="K41" s="7"/>
+        <v>315</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L41" s="4"/>
-      <c r="M41" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="N41" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="O41" s="16"/>
-      <c r="P41" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q41" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="R41" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="M41" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="N41" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q41" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R41" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G42" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I42" t="s">
-        <v>284</v>
-      </c>
-      <c r="K42" s="7"/>
+        <v>281</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="19" t="s">
-        <v>177</v>
+      <c r="M42" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q42" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="R42" s="16"/>
-    </row>
-    <row r="43" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q42" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="R42" s="15"/>
+    </row>
+    <row r="43" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G43" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I43" t="s">
-        <v>284</v>
-      </c>
-      <c r="K43" s="7"/>
+        <v>281</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L43" s="4"/>
-      <c r="M43" s="19" t="s">
-        <v>269</v>
+      <c r="M43" s="18" t="s">
+        <v>266</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="O43" s="16"/>
-      <c r="P43" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q43" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="R43" s="16"/>
-    </row>
-    <row r="44" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q43" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="R43" s="15"/>
+    </row>
+    <row r="44" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G44"/>
       <c r="H44"/>
-      <c r="I44" s="29"/>
+      <c r="I44" s="27"/>
       <c r="K44" s="7"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="34.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J45" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>3</v>
@@ -3746,564 +3913,581 @@
       <c r="L45" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M45" s="15" t="s">
-        <v>222</v>
+      <c r="M45" s="14" t="s">
+        <v>219</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="O45" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="P45" s="16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G46" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="I46" s="26"/>
+      <c r="J46" t="s">
+        <v>220</v>
+      </c>
+      <c r="K46" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="H46" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="I46" s="27"/>
-      <c r="J46" t="s">
-        <v>223</v>
-      </c>
-      <c r="K46" s="7"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="15" t="s">
-        <v>223</v>
+      <c r="M46" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="N46" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="O46" s="16" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+      <c r="O46" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="I47" s="27"/>
+        <v>302</v>
+      </c>
+      <c r="I47" s="26"/>
       <c r="J47" t="s">
         <v>4</v>
       </c>
-      <c r="K47" s="7"/>
+      <c r="K47" s="15" t="s">
+        <v>217</v>
+      </c>
       <c r="L47" s="4"/>
-      <c r="M47" s="15" t="s">
+      <c r="M47" s="14" t="s">
         <v>4</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="O47" s="16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+      <c r="O47" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J48" t="s">
-        <v>236</v>
-      </c>
-      <c r="K48" s="7"/>
+        <v>233</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>241</v>
+      </c>
       <c r="L48" s="4"/>
-      <c r="M48" s="15" t="s">
-        <v>236</v>
+      <c r="M48" s="14" t="s">
+        <v>233</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="O48" s="16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+      <c r="O48" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="F49" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="J49" t="s">
+        <v>234</v>
+      </c>
+      <c r="K49" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="J49" t="s">
-        <v>237</v>
-      </c>
-      <c r="K49" s="7"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="15" t="s">
-        <v>237</v>
+      <c r="M49" s="14" t="s">
+        <v>234</v>
       </c>
       <c r="N49" t="s">
-        <v>245</v>
-      </c>
-      <c r="O49" s="16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J50" t="s">
-        <v>238</v>
-      </c>
-      <c r="K50" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>241</v>
+      </c>
       <c r="L50" s="4"/>
-      <c r="M50" s="15" t="s">
-        <v>238</v>
+      <c r="M50" s="14" t="s">
+        <v>235</v>
       </c>
       <c r="N50" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="O50" s="16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+      <c r="O50" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J51" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K51" s="7"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="15" t="s">
-        <v>247</v>
+      <c r="M51" s="14" t="s">
+        <v>244</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="K52" s="7"/>
+        <v>286</v>
+      </c>
+      <c r="K52" s="15" t="s">
+        <v>251</v>
+      </c>
       <c r="L52" s="4"/>
-      <c r="M52" s="15" t="s">
-        <v>252</v>
+      <c r="M52" s="14" t="s">
+        <v>249</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="O52" s="16" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="O52" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="K53" s="7"/>
+        <v>287</v>
+      </c>
+      <c r="K53" s="15" t="s">
+        <v>254</v>
+      </c>
       <c r="L53" s="4"/>
-      <c r="M53" s="15" t="s">
+      <c r="M53" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="N53" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="O53" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="P53" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="N53" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="O53" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="P53" s="16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:16" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
       </c>
       <c r="F54" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="I54" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="K54" s="7"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="30.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="M54" s="14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K55" s="7"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="O55" s="16"/>
-    </row>
-    <row r="56" spans="1:16" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M55" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="O55" s="15"/>
+    </row>
+    <row r="56" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G56" s="33" t="s">
-        <v>295</v>
+        <v>53</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>292</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J56" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
-        <v>310</v>
-      </c>
-      <c r="B57" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35" t="s">
+    <row r="57" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G57" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="H57" s="35" t="s">
-        <v>311</v>
-      </c>
-      <c r="I57" s="27"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="G57" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="H57" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="I57" s="26"/>
       <c r="J57" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="L57" s="4"/>
       <c r="N57" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="O57" t="s">
-        <v>261</v>
-      </c>
-      <c r="P57" s="21" t="s">
-        <v>75</v>
+        <v>258</v>
+      </c>
+      <c r="P57" s="20" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>306</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G58" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="H58" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="I58" s="26"/>
+      <c r="J58" t="s">
+        <v>269</v>
+      </c>
+      <c r="L58" s="4"/>
+      <c r="P58" s="20"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>308</v>
+      </c>
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G59" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="B58" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" s="6" t="s">
+      <c r="I59" s="26"/>
+      <c r="L59" s="4"/>
+      <c r="P59" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="I60" s="26"/>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>55</v>
       </c>
-      <c r="G58" s="36" t="s">
-        <v>280</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>315</v>
-      </c>
-      <c r="I58" s="27"/>
-      <c r="J58" t="s">
-        <v>272</v>
-      </c>
-      <c r="L58" s="4"/>
-      <c r="P58" s="21"/>
-    </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>312</v>
-      </c>
-      <c r="B59" t="s">
-        <v>31</v>
-      </c>
-      <c r="F59" s="6" t="s">
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H61" s="35" t="s">
         <v>313</v>
       </c>
-      <c r="G59" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="I59" s="27"/>
-      <c r="L59" s="4"/>
-      <c r="P59" s="21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" t="s">
-        <v>31</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="I60" s="27"/>
-      <c r="L60" s="4"/>
-    </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" t="s">
-        <v>31</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="H61" s="37" t="s">
-        <v>317</v>
-      </c>
-      <c r="I61" s="27"/>
+      <c r="I61" s="26"/>
       <c r="L61" s="4"/>
       <c r="N61" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G62" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="I62" s="33" t="s">
-        <v>298</v>
+        <v>59</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="I62" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="K62" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="B63" t="s">
-        <v>31</v>
-      </c>
-      <c r="F63" s="6" t="s">
+      <c r="I63" s="26"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="I64" s="26"/>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="H65" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="I63" s="27"/>
-      <c r="L63" s="4"/>
-    </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="B64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="I64" s="27"/>
-      <c r="L64" s="4"/>
-    </row>
-    <row r="65" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="B65" t="s">
-        <v>31</v>
-      </c>
-      <c r="F65" s="6" t="s">
+      <c r="I65" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="G65" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="I65" s="27" t="s">
-        <v>331</v>
-      </c>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="s">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="B66" t="s">
-        <v>31</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="I66" s="27"/>
+      <c r="I66" s="26"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:16" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -4318,31 +4502,31 @@
         <v>19</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="I67" s="27"/>
+        <v>258</v>
+      </c>
+      <c r="I67" s="26"/>
       <c r="J67" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L67" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N67" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="O67" s="20" t="s">
-        <v>263</v>
-      </c>
-      <c r="P67" s="20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="O67" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="P67" s="19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -4357,28 +4541,28 @@
         <v>19</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="I68" s="27"/>
+        <v>334</v>
+      </c>
+      <c r="I68" s="26"/>
       <c r="J68" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N68" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="O68" s="24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="O68" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -4392,23 +4576,26 @@
       <c r="E69" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G69" s="39" t="s">
-        <v>333</v>
-      </c>
-      <c r="I69" s="27"/>
+      <c r="G69" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="I69" s="26"/>
       <c r="J69" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L69" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -4423,12 +4610,12 @@
         <v>19</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="I70" s="27"/>
+        <v>334</v>
+      </c>
+      <c r="I70" s="26"/>
       <c r="J70" t="s">
         <v>12</v>
       </c>
@@ -4439,15 +4626,15 @@
         <v>2</v>
       </c>
       <c r="N70" t="s">
-        <v>266</v>
-      </c>
-      <c r="O70" s="16" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="O70" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
@@ -4462,12 +4649,12 @@
         <v>19</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="I71" s="27"/>
+        <v>335</v>
+      </c>
+      <c r="I71" s="26"/>
       <c r="J71" t="s">
         <v>0</v>
       </c>
@@ -4478,9 +4665,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
@@ -4495,12 +4682,12 @@
         <v>19</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="I72" s="27"/>
+        <v>335</v>
+      </c>
+      <c r="I72" s="26"/>
       <c r="J72" t="s">
         <v>6</v>
       </c>
@@ -4511,148 +4698,155 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I73" s="27"/>
-      <c r="P73" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I73" s="26"/>
+      <c r="P73" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
-      <c r="E74" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="F74" s="23" t="s">
+      <c r="E74" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F74" s="22" t="s">
         <v>12</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="I74" s="30"/>
-    </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="I74" s="28"/>
+      <c r="K74" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
       </c>
-      <c r="E75" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="F75" s="23" t="s">
+      <c r="E75" s="21" t="s">
         <v>213</v>
       </c>
+      <c r="F75" s="22" t="s">
+        <v>210</v>
+      </c>
       <c r="G75" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="I75" s="30"/>
-    </row>
-    <row r="76" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="I75" s="28"/>
+    </row>
+    <row r="76" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
       </c>
-      <c r="E76" s="22" t="s">
+      <c r="E76" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F76" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="G76" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="H76" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="I76" s="28"/>
+    </row>
+    <row r="77" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>216</v>
-      </c>
-      <c r="F76" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="G76" s="39" t="s">
-        <v>333</v>
-      </c>
-      <c r="H76" s="23"/>
-      <c r="I76" s="30"/>
-    </row>
-    <row r="77" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>219</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
-      <c r="E77" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="F77" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="G77" s="39" t="s">
-        <v>333</v>
-      </c>
-      <c r="H77" s="23"/>
-      <c r="I77" s="30"/>
-    </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="G77" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="H77" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="I77" s="28"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" t="s">
+        <v>62</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I78" s="26"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79" t="s">
+        <v>62</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I79" s="26"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>65</v>
       </c>
-      <c r="B78" t="s">
-        <v>64</v>
-      </c>
-      <c r="F78" s="6" t="s">
+      <c r="B80" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I78" s="27"/>
-    </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="I80" s="26"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>66</v>
       </c>
-      <c r="B79" t="s">
-        <v>64</v>
-      </c>
-      <c r="F79" s="6" t="s">
+      <c r="B81" t="s">
+        <v>62</v>
+      </c>
+      <c r="F81" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I79" s="27"/>
-    </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" t="s">
-        <v>64</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I80" s="27"/>
-    </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>68</v>
-      </c>
-      <c r="B81" t="s">
-        <v>64</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I81" s="27"/>
+      <c r="I81" s="26"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L72">
@@ -4721,6 +4915,85 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEDD958-2C6B-48A3-8B65-9D45041E808A}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="42.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.140625" style="38" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>